<commit_message>
for rechecking face mapping of masara
</commit_message>
<xml_diff>
--- a/FACE_MAPPING_GIS/MAS-BBK for xyz/L496 MAS 41S ODW - XY OK/496_MAS_41S_ODW.xlsx
+++ b/FACE_MAPPING_GIS/MAS-BBK for xyz/L496 MAS 41S ODW - XY OK/496_MAS_41S_ODW.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\01 AMCI Project\4 Geology\005 GIS\Database\2021 Database Monitoring\2022\FACEMAPPING P 2022\MAS-BBK for xyz\L496 MAS 41S ODW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcmadarang\Documents\Current Work\R_projects\BLOCKING_GIS_2\FACE_MAPPING_GIS\MAS-BBK for xyz\L496 MAS 41S ODW - XY OK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF7CD0E-43EA-4647-9105-5190AFA7B5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F99FC6-368E-4C05-BB67-768549B767CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34515" yWindow="480" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HEADER" sheetId="1" r:id="rId1"/>
     <sheet name="ORIG_ASSAY" sheetId="2" r:id="rId2"/>
     <sheet name="SURVEY" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="Z_9C1D411A_E240_49DF_88C0_6B2303C52A25_.wvu.Cols" localSheetId="1" hidden="1">ORIG_ASSAY!$M:$N</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
+  <customWorkbookViews>
+    <customWorkbookView name="Mark C. Madarang - Personal View" guid="{9C1D411A-E240-49DF-88C0-6B2303C52A25}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+  </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="282">
   <si>
     <t>HOLE-ID</t>
   </si>
@@ -877,6 +883,9 @@
   </si>
   <si>
     <t>MAS_496_41S_W_052</t>
+  </si>
+  <si>
+    <t>pasdads</t>
   </si>
 </sst>
 </file>
@@ -1347,6 +1356,26 @@
 </styleSheet>
 </file>
 
+<file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{EA55D9DF-9CC9-4DEF-A7C4-0A59E1A0D703}">
+  <header guid="{EA55D9DF-9CC9-4DEF-A7C4-0A59E1A0D703}" dateTime="2022-07-11T15:07:17" maxSheetId="4" userName="Mark C. Madarang" r:id="rId1">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
+</headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1671,8 +1700,8 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2784,7 +2813,7 @@
         <v>44436</v>
       </c>
       <c r="K34" s="27" t="s">
-        <v>28</v>
+        <v>281</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -3342,9 +3371,17 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K9">
     <sortCondition ref="A2"/>
   </sortState>
+  <customSheetViews>
+    <customSheetView guid="{9C1D411A-E240-49DF-88C0-6B2303C52A25}">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K34" sqref="K34"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+  </customSheetViews>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3353,8 +3390,8 @@
   <dimension ref="A1:W219"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O175" sqref="O175"/>
+      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B147" sqref="B147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12114,8 +12151,16 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W35">
     <sortCondition ref="A2"/>
   </sortState>
+  <customSheetViews>
+    <customSheetView guid="{9C1D411A-E240-49DF-88C0-6B2303C52A25}" hiddenColumns="1">
+      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B147" sqref="B147"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+  </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -13738,8 +13783,16 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D19">
     <sortCondition ref="A2"/>
   </sortState>
+  <customSheetViews>
+    <customSheetView guid="{9C1D411A-E240-49DF-88C0-6B2303C52A25}">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K54" sqref="K54"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="8" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+  </customSheetViews>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="8" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>